<commit_message>
add HHV to components
</commit_message>
<xml_diff>
--- a/exposan/g2rt/data/impact_items.xlsx
+++ b/exposan/g2rt/data/impact_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zixuanwang/Library/CloudStorage/GoogleDrive-wyatt4428@gmail.com/My Drive/4- Research/430- UIUC/433. Coding/QSD_san/EXPOsan/exposan/g2rt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75D638D-DF09-054B-89B5-BDE26D7D3D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A578B6D3-E10C-1649-B9C8-F7E60509A249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="-2440" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="36">
   <si>
     <t>uniform</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Compressor_300kW</t>
+  </si>
+  <si>
+    <t>ZincCoat</t>
   </si>
 </sst>
 </file>
@@ -517,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -681,6 +684,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -688,10 +699,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28627DAA-889C-6942-A3B5-3C8A993554C1}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="290" zoomScaleNormal="290" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -735,11 +746,11 @@
         <v>8.8785325999999998</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D19" si="0">C2*0.9</f>
+        <f t="shared" ref="D2:D20" si="0">C2*0.9</f>
         <v>7.9906793399999998</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E19" si="1">C2*1.1</f>
+        <f t="shared" ref="E2:E20" si="1">C2*1.1</f>
         <v>9.7663858599999998</v>
       </c>
       <c r="F2" t="s">
@@ -1171,7 +1182,32 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>5.4322602</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>4.8890341800000003</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>5.9754862200000005</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1182,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AFA65E-2AB0-4D0E-8E5A-9EA8A54DBEB2}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1668,6 +1704,31 @@
         <v>23</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>0.12593618000000001</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20" si="2">C20*0.9</f>
+        <v>0.11334256200000001</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20" si="3">C20*1.1</f>
+        <v>0.13852979800000001</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1676,9 +1737,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338397C7-E99F-4EAF-BD45-82C00ACD803A}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -2162,6 +2223,31 @@
         <v>23</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>0.39828018999999998</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20" si="2">C20*0.9</f>
+        <v>0.35845217099999999</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20" si="3">C20*1.1</f>
+        <v>0.43810820900000003</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2169,10 +2255,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA7D3C9-542A-47E5-A276-0B7825A720DE}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A12" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2655,6 +2741,31 @@
         <v>23</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>0.33182298999999998</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20" si="2">C20*0.9</f>
+        <v>0.29864069100000001</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20" si="3">C20*1.1</f>
+        <v>0.36500528900000001</v>
+      </c>
+      <c r="F20" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add combustor unit with energy recovery
</commit_message>
<xml_diff>
--- a/exposan/g2rt/data/impact_items.xlsx
+++ b/exposan/g2rt/data/impact_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zixuanwang/Library/CloudStorage/GoogleDrive-wyatt4428@gmail.com/My Drive/4- Research/430- UIUC/433. Coding/QSD_san/EXPOsan/exposan/g2rt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A578B6D3-E10C-1649-B9C8-F7E60509A249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B74C3F8-BFD1-D043-AD8A-97FE160CBF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="34560" yWindow="-2440" windowWidth="51200" windowHeight="28300" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="38">
   <si>
     <t>uniform</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>ZincCoat</t>
+  </si>
+  <si>
+    <t>WoodPellet</t>
+  </si>
+  <si>
+    <t>StoneWool</t>
   </si>
 </sst>
 </file>
@@ -520,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,6 +698,22 @@
         <v>32</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -699,10 +721,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28627DAA-889C-6942-A3B5-3C8A993554C1}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="290" zoomScaleNormal="290" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A14" zoomScale="290" zoomScaleNormal="290" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,11 +768,11 @@
         <v>8.8785325999999998</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D20" si="0">C2*0.9</f>
+        <f t="shared" ref="D2:D22" si="0">C2*0.9</f>
         <v>7.9906793399999998</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E20" si="1">C2*1.1</f>
+        <f t="shared" ref="E2:E22" si="1">C2*1.1</f>
         <v>9.7663858599999998</v>
       </c>
       <c r="F2" t="s">
@@ -1207,6 +1229,56 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>0.14178389</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.12760550100000001</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0.15596227900000001</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>1.2681741</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1.1413566900000001</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>1.3949915100000001</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1218,10 +1290,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45AFA65E-2AB0-4D0E-8E5A-9EA8A54DBEB2}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A3" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1715,17 +1787,67 @@
         <v>0.12593618000000001</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20" si="2">C20*0.9</f>
+        <f t="shared" ref="D20:D22" si="2">C20*0.9</f>
         <v>0.11334256200000001</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E20" si="3">C20*1.1</f>
+        <f t="shared" ref="E20:E22" si="3">C20*1.1</f>
         <v>0.13852979800000001</v>
       </c>
       <c r="F20" t="s">
         <v>0</v>
       </c>
       <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>4.3958951000000003E-2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>3.9563055900000005E-2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>4.8354846100000008E-2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>2.7597746999999999E-2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>2.48379723E-2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>3.0357521700000001E-2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1737,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338397C7-E99F-4EAF-BD45-82C00ACD803A}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A3" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2234,17 +2356,67 @@
         <v>0.39828018999999998</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20" si="2">C20*0.9</f>
+        <f t="shared" ref="D20:D22" si="2">C20*0.9</f>
         <v>0.35845217099999999</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E20" si="3">C20*1.1</f>
+        <f t="shared" ref="E20:E22" si="3">C20*1.1</f>
         <v>0.43810820900000003</v>
       </c>
       <c r="F20" t="s">
         <v>0</v>
       </c>
       <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>6.8199964000000002E-3</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>6.1379967600000002E-3</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>7.5019960400000011E-3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>5.9336112000000003E-2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>5.3402500800000002E-2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>6.5269723200000004E-2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2255,10 +2427,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA7D3C9-542A-47E5-A276-0B7825A720DE}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView topLeftCell="A12" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2752,17 +2924,67 @@
         <v>0.33182298999999998</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20" si="2">C20*0.9</f>
+        <f t="shared" ref="D20:D22" si="2">C20*0.9</f>
         <v>0.29864069100000001</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E20" si="3">C20*1.1</f>
+        <f t="shared" ref="E20:E22" si="3">C20*1.1</f>
         <v>0.36500528900000001</v>
       </c>
       <c r="F20" t="s">
         <v>0</v>
       </c>
       <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>6.172004E-3</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>5.5548035999999999E-3</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>6.7892044000000002E-3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>5.1289876999999998E-2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>4.6160889300000001E-2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>5.6418864700000002E-2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update RO unit & impact item
</commit_message>
<xml_diff>
--- a/exposan/g2rt/data/impact_items.xlsx
+++ b/exposan/g2rt/data/impact_items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zixuanwang/Library/CloudStorage/GoogleDrive-wyatt4428@gmail.com/My Drive/4- Research/430- UIUC/433. Coding/QSD_san/EXPOsan/exposan/g2rt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA5C794-BE13-3A4D-9D2C-7CFE7B8AA51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A027B3C8-A51A-2A44-8525-4CAE4253AF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28627DAA-889C-6942-A3B5-3C8A993554C1}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>